<commit_message>
modified and updated model compaison table
</commit_message>
<xml_diff>
--- a/research/uc_berkeley/datasci203/test_variable_selection.xlsx
+++ b/research/uc_berkeley/datasci203/test_variable_selection.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UCB\202508FALL\DATASCI203\gitRepo\MattKimolu\research\uc_berkeley\datasci203\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{44C69E4F-9C93-4875-9E9A-316F42AB37F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93724C1-A055-4CA4-8411-D362BB8C3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{85824CA9-CD63-4BB5-9A8A-A27D6984C2E2}"/>
   </bookViews>
   <sheets>
     <sheet name="test_variable_selection" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_variable_selection!$A$1:$AO$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_variable_selection!$A$1:$AO$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>p</t>
   </si>
@@ -629,11 +630,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1012,7 +1014,7 @@
   <dimension ref="A1:AO22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1021,7 +1023,7 @@
     <col min="37" max="37" width="13.26953125" customWidth="1"/>
     <col min="38" max="38" width="11.1796875" customWidth="1"/>
     <col min="39" max="39" width="10.453125" customWidth="1"/>
-    <col min="40" max="40" width="10.7265625" customWidth="1"/>
+    <col min="40" max="40" width="10.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
@@ -1267,7 +1269,7 @@
       <c r="AM2">
         <v>0.79073589454545701</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="2">
         <v>2113771.7341743298</v>
       </c>
       <c r="AO2">
@@ -1392,7 +1394,7 @@
       <c r="AM3">
         <v>0.79437848976677605</v>
       </c>
-      <c r="AN3">
+      <c r="AN3" s="2">
         <v>2076977.96679059</v>
       </c>
       <c r="AO3">
@@ -1517,7 +1519,7 @@
       <c r="AM4">
         <v>0.79658851328857105</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="2">
         <v>2054654.57194901</v>
       </c>
       <c r="AO4">
@@ -1642,7 +1644,7 @@
       <c r="AM5">
         <v>0.79758114397406998</v>
       </c>
-      <c r="AN5">
+      <c r="AN5" s="2">
         <v>2044628.03308835</v>
       </c>
       <c r="AO5">
@@ -1767,7 +1769,7 @@
       <c r="AM6">
         <v>0.79945988674557</v>
       </c>
-      <c r="AN6">
+      <c r="AN6" s="2">
         <v>2025650.89719801</v>
       </c>
       <c r="AO6">
@@ -1892,7 +1894,7 @@
       <c r="AM7">
         <v>0.79902723231924899</v>
       </c>
-      <c r="AN7">
+      <c r="AN7" s="2">
         <v>2030021.1292310499</v>
       </c>
       <c r="AO7">
@@ -2017,7 +2019,7 @@
       <c r="AM8">
         <v>0.79958689515117898</v>
       </c>
-      <c r="AN8">
+      <c r="AN8" s="2">
         <v>2024367.98832458</v>
       </c>
       <c r="AO8">
@@ -2142,7 +2144,7 @@
       <c r="AM9">
         <v>0.79935187021219101</v>
       </c>
-      <c r="AN9">
+      <c r="AN9" s="2">
         <v>2026741.9696233701</v>
       </c>
       <c r="AO9">
@@ -2267,7 +2269,7 @@
       <c r="AM10">
         <v>0.79777982564772398</v>
       </c>
-      <c r="AN10">
+      <c r="AN10" s="2">
         <v>2042621.1542451901</v>
       </c>
       <c r="AO10">
@@ -2392,7 +2394,7 @@
       <c r="AM11">
         <v>0.795531620579504</v>
       </c>
-      <c r="AN11">
+      <c r="AN11" s="2">
         <v>2065330.2199758301</v>
       </c>
       <c r="AO11">
@@ -2517,7 +2519,7 @@
       <c r="AM12">
         <v>0.79150302152385199</v>
       </c>
-      <c r="AN12">
+      <c r="AN12" s="2">
         <v>2106023.0028764801</v>
       </c>
       <c r="AO12">
@@ -2642,7 +2644,7 @@
       <c r="AM13">
         <v>0.79144129285424802</v>
       </c>
-      <c r="AN13">
+      <c r="AN13" s="2">
         <v>2106646.5226947102</v>
       </c>
       <c r="AO13">
@@ -2767,7 +2769,7 @@
       <c r="AM14">
         <v>0.788762910899243</v>
       </c>
-      <c r="AN14">
+      <c r="AN14" s="2">
         <v>2133700.7948906799</v>
       </c>
       <c r="AO14">
@@ -2892,7 +2894,7 @@
       <c r="AM15">
         <v>0.77927089080482304</v>
       </c>
-      <c r="AN15">
+      <c r="AN15" s="2">
         <v>2229579.4632949801</v>
       </c>
       <c r="AO15">
@@ -3017,7 +3019,7 @@
       <c r="AM16">
         <v>0.76965668061605896</v>
       </c>
-      <c r="AN16">
+      <c r="AN16" s="2">
         <v>2326692.3709256402</v>
       </c>
       <c r="AO16">
@@ -3142,7 +3144,7 @@
       <c r="AM17">
         <v>0.76135072522908898</v>
       </c>
-      <c r="AN17">
+      <c r="AN17" s="2">
         <v>2410590.6280307299</v>
       </c>
       <c r="AO17">
@@ -3267,7 +3269,7 @@
       <c r="AM18">
         <v>0.74269377331824804</v>
       </c>
-      <c r="AN18">
+      <c r="AN18" s="2">
         <v>2599044.0539506902</v>
       </c>
       <c r="AO18">
@@ -3392,7 +3394,7 @@
       <c r="AM19">
         <v>0.72441967351029701</v>
       </c>
-      <c r="AN19">
+      <c r="AN19" s="2">
         <v>2783630.2999178399</v>
       </c>
       <c r="AO19">
@@ -3517,7 +3519,7 @@
       <c r="AM20">
         <v>0.71022092354404298</v>
       </c>
-      <c r="AN20">
+      <c r="AN20" s="2">
         <v>2927051.5344104199</v>
       </c>
       <c r="AO20">
@@ -3642,7 +3644,7 @@
       <c r="AM21">
         <v>0.68854606616228198</v>
       </c>
-      <c r="AN21">
+      <c r="AN21" s="2">
         <v>3145988.7514563701</v>
       </c>
       <c r="AO21">
@@ -3767,7 +3769,7 @@
       <c r="AM22">
         <v>0.27512736952405997</v>
       </c>
-      <c r="AN22">
+      <c r="AN22" s="2">
         <v>7321921.13811641</v>
       </c>
       <c r="AO22">
@@ -3775,11 +3777,234 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO1" xr:uid="{5911436D-5D3E-4A27-B89B-98AD96121D8E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO22">
-      <sortCondition descending="1" ref="AL1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AO22" xr:uid="{5911436D-5D3E-4A27-B89B-98AD96121D8E}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8473C759-912E-4A3F-A305-7FA595119661}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>94514110.309654295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>0.85604725555806604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <v>0.79658851328857105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2054654.57194901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>7.7866897329426301</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>